<commit_message>
ad checkbox print and some details
</commit_message>
<xml_diff>
--- a/LogItems_test.xlsx
+++ b/LogItems_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\herma\stack\Python\productiebonnen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA37A612-139F-45A4-9F7E-4EF599EACFDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C287A1FE-0E5D-406B-BC2C-2B3EAD3110C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$14</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="6">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -40,25 +40,7 @@
     <t>X252</t>
   </si>
   <si>
-    <t>1001002</t>
-  </si>
-  <si>
-    <t>Mok met naam</t>
-  </si>
-  <si>
-    <t>175° - 180 sec</t>
-  </si>
-  <si>
-    <t>1001004</t>
-  </si>
-  <si>
     <t>Klassieke Foto Mok</t>
-  </si>
-  <si>
-    <t>20/40</t>
-  </si>
-  <si>
-    <t>100/100</t>
   </si>
 </sst>
 </file>
@@ -119,9 +101,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -436,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6B9C2A6-FF5F-4F5A-B740-0D995DBAD324}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E162"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -469,34 +449,1296 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
+      <c r="A2" s="3">
+        <v>1001011</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>8</v>
+      <c r="A3" s="3">
+        <v>1001014</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" t="s">
-        <v>11</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>1001022</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>1001036</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <v>1001037</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>1001038</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <v>1001039</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <v>1001040</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <v>1001041</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <v>1001042</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
+        <v>1001043</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
+        <v>1001044</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <v>1001045</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
+        <v>1001046</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
+        <v>1001047</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <v>1001048</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
+        <v>1014301</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
+        <v>1033105</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
+        <v>1035701</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="3">
+        <v>1038201</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="3">
+        <v>1043901</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="3">
+        <v>1043902</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
+        <v>1043904</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="3">
+        <v>1044201</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="3">
+        <v>1045401</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="3">
+        <v>1046201</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="3">
+        <v>1049401</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="3">
+        <v>1049501</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="3">
+        <v>1049702</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="3">
+        <v>1059701</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="3">
+        <v>1070501</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="3">
+        <v>1070901</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="3">
+        <v>1093861</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="3">
+        <v>2015201</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="3">
+        <v>2023601</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="3">
+        <v>2023801</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="3">
+        <v>2028501</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="3">
+        <v>2029901</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="3">
+        <v>2053402</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="3">
+        <v>2056001</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="3">
+        <v>2081101</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="3">
+        <v>2081201</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="3">
+        <v>2105101</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="3">
+        <v>2105201</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="3">
+        <v>3000801</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="3">
+        <v>3000901</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" s="3">
+        <v>3001322</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="3">
+        <v>3001422</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="3">
+        <v>3001522</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="3">
+        <v>3001722</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="3">
+        <v>3015001</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="3">
+        <v>3015101</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" s="3">
+        <v>3015201</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" s="3">
+        <v>3015301</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" s="3">
+        <v>3015401</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" s="3">
+        <v>3015501</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" s="3">
+        <v>3016001</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" s="3">
+        <v>3016101</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" s="3">
+        <v>3016201</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" s="3">
+        <v>3016301</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" s="3">
+        <v>3016401</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" s="3">
+        <v>3016501</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" s="3">
+        <v>3021102</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" s="3">
+        <v>3021302</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" s="3">
+        <v>3021402</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" s="3">
+        <v>3021502</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" s="3">
+        <v>3021602</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" s="3">
+        <v>3021702</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" s="3">
+        <v>3021802</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" s="3">
+        <v>3022301</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" s="3">
+        <v>3046001</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" s="3">
+        <v>3046101</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" s="3">
+        <v>3046201</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" s="3">
+        <v>3046301</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" s="3">
+        <v>3046401</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" s="3">
+        <v>3046501</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" s="3">
+        <v>3046601</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" s="3">
+        <v>3046701</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" s="3">
+        <v>3074901</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" s="3">
+        <v>3075001</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" s="3">
+        <v>3075201</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" s="3">
+        <v>3078301</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" s="3">
+        <v>3078501</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" s="3">
+        <v>3084701</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" s="3">
+        <v>3312501</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" s="3">
+        <v>4048201</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" s="3">
+        <v>4048261</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" s="3">
+        <v>4056101</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" s="3">
+        <v>4056601</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" s="3">
+        <v>4059401</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" s="3">
+        <v>4063802</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" s="3">
+        <v>4063902</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" s="3">
+        <v>4065361</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" s="3">
+        <v>4065901</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" s="3">
+        <v>4066901</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" s="3">
+        <v>4100101</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" s="3">
+        <v>4100849</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" s="3">
+        <v>4102449</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" s="3">
+        <v>4102549</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" s="3">
+        <v>4104202</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" s="3">
+        <v>4104204</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103" s="3">
+        <v>4104208</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" s="3">
+        <v>4104349</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105" s="3">
+        <v>4104449</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106" s="3">
+        <v>4104949</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107" s="3">
+        <v>4105049</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108" s="3">
+        <v>4105149</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109" s="3">
+        <v>4121302</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110" s="3">
+        <v>4121303</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111" s="3">
+        <v>4121304</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112" s="3">
+        <v>4121306</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113" s="3">
+        <v>4121307</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114" s="3">
+        <v>4165401</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115" s="3">
+        <v>4165901</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116" s="3">
+        <v>4176601</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117" s="3">
+        <v>5006001</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118" s="3">
+        <v>5009301</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119" s="3">
+        <v>5010602</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120" s="3">
+        <v>5011802</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121" s="3">
+        <v>5011902</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122" s="3">
+        <v>5012002</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A123" s="3">
+        <v>5048361</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124" s="3">
+        <v>5048801</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125" s="3">
+        <v>5049001</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126" s="3">
+        <v>5049002</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127" s="3">
+        <v>5049861</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128" s="3">
+        <v>5050301</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129" s="3">
+        <v>5071602</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130" s="3">
+        <v>5072101</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131" s="3">
+        <v>5080001</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132" s="3">
+        <v>5100501</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133" s="3">
+        <v>5101801</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A134" s="3">
+        <v>5101904</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135" s="3">
+        <v>5102101</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A136" s="3">
+        <v>5102201</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A137" s="3">
+        <v>5102301</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A138" s="3">
+        <v>5102501</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A139" s="3">
+        <v>5102502</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A140" s="3">
+        <v>5102506</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A141" s="3">
+        <v>5102701</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A142" s="3">
+        <v>5106001</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A143" s="3">
+        <v>5121201</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A144" s="3">
+        <v>5121202</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A145" s="3">
+        <v>5121203</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A146" s="3">
+        <v>5121204</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A147" s="3">
+        <v>5121205</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A148" s="3">
+        <v>5121206</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A149" s="3">
+        <v>5121207</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A150" s="3">
+        <v>5150402</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A151" s="3">
+        <v>5201001</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A152" s="3">
+        <v>7777001</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A153" s="3">
+        <v>9011001</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A154" s="3">
+        <v>9011002</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A155" s="3">
+        <v>9011003</v>
+      </c>
+      <c r="B155" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A156" s="3">
+        <v>9011004</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A157" s="3">
+        <v>9011005</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A158" s="3">
+        <v>9011006</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A159" s="3">
+        <v>9011007</v>
+      </c>
+      <c r="B159" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A160" s="3">
+        <v>9011008</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A161" s="3">
+        <v>9011009</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A162" s="3">
+        <v>9011011</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F452">
-    <sortCondition ref="A2:A452"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F449">
+    <sortCondition ref="A2:A449"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>

</xml_diff>